<commit_message>
feat: threading support; save/restore cookie for chrome driver
</commit_message>
<xml_diff>
--- a/result.xlsx
+++ b/result.xlsx
@@ -13,83 +13,10 @@
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
-  <si>
-    <t>S00001</t>
-  </si>
-  <si>
-    <t>S00002</t>
-  </si>
-  <si>
-    <t>S00004</t>
-  </si>
-  <si>
-    <t>无锡明宇机械有限公司</t>
-  </si>
-  <si>
-    <t>上海宝富汽车部件有限公司</t>
-  </si>
-  <si>
-    <t>内江金鸿曲轴有限公司</t>
-  </si>
-  <si>
-    <t>江苏省无锡市惠山区洛社镇新开河村</t>
-  </si>
-  <si>
-    <t>上海市宝山区杨宗路205号</t>
-  </si>
-  <si>
-    <t>四川省内江市汉渝大道1558号（641000）</t>
-  </si>
-  <si>
-    <t>陆丽</t>
-  </si>
-  <si>
-    <t>孟燕</t>
-  </si>
-  <si>
-    <t>付好</t>
-  </si>
-  <si>
-    <t>0510-83831285</t>
-  </si>
-  <si>
-    <t>15026717209</t>
-  </si>
-  <si>
-    <t xml:space="preserve">无锡市惠山区洛社镇新开河村  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">上海市宝山区杨宗路205号  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">内江市市中区汉渝大道1558号  </t>
-  </si>
-  <si>
-    <t>0.839</t>
-  </si>
-  <si>
-    <t>0.929</t>
-  </si>
-  <si>
-    <t>0.600</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <fonts count="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -105,7 +32,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -113,30 +40,12 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -431,117 +340,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:8">
-      <c r="A1" s="1">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G2" t="s">
-        <v>14</v>
-      </c>
-      <c r="H2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F3" t="s">
-        <v>13</v>
-      </c>
-      <c r="G3" t="s">
-        <v>15</v>
-      </c>
-      <c r="H3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F4">
-        <v>15884862273</v>
-      </c>
-      <c r="G4" t="s">
-        <v>16</v>
-      </c>
-      <c r="H4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>